<commit_message>
run TM on PDFs
</commit_message>
<xml_diff>
--- a/results/relevant_papers.xlsx
+++ b/results/relevant_papers.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latifa\Documents\Um6p\Survey\Survey\sci-scraper\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B92D0A4-B190-4E5F-A1F3-0D736BFA323E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="443">
   <si>
     <t>Title</t>
   </si>
@@ -1356,8 +1362,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1381,12 +1387,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1420,12 +1432,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1433,13 +1446,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1477,7 +1498,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1511,6 +1532,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1545,9 +1567,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1720,16 +1743,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="66" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,11 +1775,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C2" t="s">
@@ -1769,7 +1795,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1789,11 +1815,11 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C4" t="s">
@@ -1809,11 +1835,11 @@
         <v>340</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C5" t="s">
@@ -1829,11 +1855,11 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C6" t="s">
@@ -1849,11 +1875,11 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>116</v>
       </c>
       <c r="C7" t="s">
@@ -1869,11 +1895,11 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C8" t="s">
@@ -1889,11 +1915,11 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C9" t="s">
@@ -1909,7 +1935,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1929,11 +1955,11 @@
         <v>346</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C11" t="s">
@@ -1949,11 +1975,11 @@
         <v>347</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C12" t="s">
@@ -1969,11 +1995,11 @@
         <v>348</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C13" t="s">
@@ -1989,7 +2015,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2009,11 +2035,11 @@
         <v>350</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C15" t="s">
@@ -2029,11 +2055,11 @@
         <v>351</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C16" t="s">
@@ -2049,11 +2075,11 @@
         <v>352</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C17" t="s">
@@ -2069,11 +2095,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C18" t="s">
@@ -2089,11 +2115,11 @@
         <v>354</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C19" t="s">
@@ -2109,7 +2135,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2129,11 +2155,11 @@
         <v>356</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>130</v>
       </c>
       <c r="C21" t="s">
@@ -2149,7 +2175,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2169,11 +2195,11 @@
         <v>358</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C23" t="s">
@@ -2189,11 +2215,11 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C24" t="s">
@@ -2209,11 +2235,11 @@
         <v>360</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>134</v>
       </c>
       <c r="C25" t="s">
@@ -2229,11 +2255,11 @@
         <v>361</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C26" t="s">
@@ -2249,7 +2275,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2269,11 +2295,11 @@
         <v>363</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>137</v>
       </c>
       <c r="C28" t="s">
@@ -2289,11 +2315,11 @@
         <v>364</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C29" t="s">
@@ -2309,7 +2335,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2329,11 +2355,11 @@
         <v>366</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C31" t="s">
@@ -2349,11 +2375,11 @@
         <v>367</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C32" t="s">
@@ -2369,11 +2395,11 @@
         <v>368</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C33" t="s">
@@ -2389,11 +2415,11 @@
         <v>369</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>143</v>
       </c>
       <c r="C34" t="s">
@@ -2409,11 +2435,11 @@
         <v>370</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C35" t="s">
@@ -2429,7 +2455,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2449,7 +2475,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2469,11 +2495,11 @@
         <v>373</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>147</v>
       </c>
       <c r="C38" t="s">
@@ -2489,11 +2515,11 @@
         <v>374</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C39" t="s">
@@ -2509,11 +2535,11 @@
         <v>375</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>149</v>
       </c>
       <c r="C40" t="s">
@@ -2529,7 +2555,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2549,7 +2575,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2569,7 +2595,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2589,7 +2615,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2609,7 +2635,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2629,7 +2655,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2649,7 +2675,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2669,7 +2695,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2689,7 +2715,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2709,7 +2735,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -2729,7 +2755,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -2749,7 +2775,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -2769,7 +2795,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -2789,7 +2815,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2809,7 +2835,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2829,7 +2855,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2849,7 +2875,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -2869,7 +2895,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -2889,7 +2915,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2909,7 +2935,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -2929,7 +2955,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2949,7 +2975,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2969,7 +2995,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2989,7 +3015,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -3009,7 +3035,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -3029,7 +3055,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -3049,7 +3075,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -3069,7 +3095,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -3089,7 +3115,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -3109,7 +3135,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -3129,7 +3155,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3149,7 +3175,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -3169,7 +3195,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -3189,7 +3215,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -3209,7 +3235,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -3229,7 +3255,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -3249,7 +3275,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -3269,7 +3295,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -3289,7 +3315,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -3309,7 +3335,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -3329,7 +3355,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -3349,7 +3375,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -3369,7 +3395,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -3389,7 +3415,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -3409,7 +3435,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -3429,7 +3455,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -3449,7 +3475,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -3469,7 +3495,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -3489,7 +3515,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -3509,7 +3535,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -3529,7 +3555,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -3549,7 +3575,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -3569,7 +3595,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -3589,7 +3615,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -3609,7 +3635,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -3629,7 +3655,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3649,7 +3675,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -3669,7 +3695,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -3689,7 +3715,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -3709,7 +3735,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -3729,7 +3755,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -3749,7 +3775,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -3769,7 +3795,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -3789,7 +3815,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -3809,7 +3835,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -3829,7 +3855,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -3851,111 +3877,111 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
-    <hyperlink ref="B64" r:id="rId63"/>
-    <hyperlink ref="B65" r:id="rId64"/>
-    <hyperlink ref="B66" r:id="rId65"/>
-    <hyperlink ref="B67" r:id="rId66"/>
-    <hyperlink ref="B68" r:id="rId67"/>
-    <hyperlink ref="B69" r:id="rId68"/>
-    <hyperlink ref="B70" r:id="rId69"/>
-    <hyperlink ref="B71" r:id="rId70"/>
-    <hyperlink ref="B72" r:id="rId71"/>
-    <hyperlink ref="B73" r:id="rId72"/>
-    <hyperlink ref="B74" r:id="rId73"/>
-    <hyperlink ref="B75" r:id="rId74"/>
-    <hyperlink ref="B76" r:id="rId75"/>
-    <hyperlink ref="B77" r:id="rId76"/>
-    <hyperlink ref="B78" r:id="rId77"/>
-    <hyperlink ref="B79" r:id="rId78"/>
-    <hyperlink ref="B80" r:id="rId79"/>
-    <hyperlink ref="B81" r:id="rId80"/>
-    <hyperlink ref="B82" r:id="rId81"/>
-    <hyperlink ref="B83" r:id="rId82"/>
-    <hyperlink ref="B84" r:id="rId83"/>
-    <hyperlink ref="B85" r:id="rId84"/>
-    <hyperlink ref="B86" r:id="rId85"/>
-    <hyperlink ref="B87" r:id="rId86"/>
-    <hyperlink ref="B88" r:id="rId87"/>
-    <hyperlink ref="B89" r:id="rId88"/>
-    <hyperlink ref="B90" r:id="rId89"/>
-    <hyperlink ref="B91" r:id="rId90"/>
-    <hyperlink ref="B92" r:id="rId91"/>
-    <hyperlink ref="B93" r:id="rId92"/>
-    <hyperlink ref="B94" r:id="rId93"/>
-    <hyperlink ref="B95" r:id="rId94"/>
-    <hyperlink ref="B96" r:id="rId95"/>
-    <hyperlink ref="B97" r:id="rId96"/>
-    <hyperlink ref="B98" r:id="rId97"/>
-    <hyperlink ref="B99" r:id="rId98"/>
-    <hyperlink ref="B100" r:id="rId99"/>
-    <hyperlink ref="B101" r:id="rId100"/>
-    <hyperlink ref="B102" r:id="rId101"/>
-    <hyperlink ref="B103" r:id="rId102"/>
-    <hyperlink ref="B104" r:id="rId103"/>
-    <hyperlink ref="B105" r:id="rId104"/>
-    <hyperlink ref="B106" r:id="rId105"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B105" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B106" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>